<commit_message>
nominas nuevas + db(order_by y limit)
</commit_message>
<xml_diff>
--- a/1DAM/F.O.L/calculo_nomina.xlsx
+++ b/1DAM/F.O.L/calculo_nomina.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alberto\Documents\ies-federica-montseny\1DAM\F.O.L\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{314C4C1E-3F4A-4643-9557-1885F9132DCA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9819DE2B-405C-4172-81BD-0234BBA1AEC1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{FD6F1533-AABF-414C-8653-F0AF724C1F26}"/>
+    <workbookView xWindow="11988" yWindow="72" windowWidth="11040" windowHeight="8964" activeTab="1" xr2:uid="{FD6F1533-AABF-414C-8653-F0AF724C1F26}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="40">
   <si>
     <t>Salario base</t>
   </si>
@@ -76,12 +76,6 @@
     <t>Complementos salariales</t>
   </si>
   <si>
-    <t>Plus Distancia</t>
-  </si>
-  <si>
-    <t>Complemento personal</t>
-  </si>
-  <si>
     <t>Horas extraordinarias</t>
   </si>
   <si>
@@ -146,6 +140,21 @@
   </si>
   <si>
     <t>LIQUIDO TOTAL A PERCIBIR</t>
+  </si>
+  <si>
+    <t>Antigüedad</t>
+  </si>
+  <si>
+    <t>Plus de idiomas</t>
+  </si>
+  <si>
+    <t>Plus de productividad</t>
+  </si>
+  <si>
+    <t>Plus idiomas</t>
+  </si>
+  <si>
+    <t>Plus Productividad</t>
   </si>
 </sst>
 </file>
@@ -566,7 +575,7 @@
   <dimension ref="C2:F16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -588,38 +597,40 @@
       </c>
       <c r="D3" s="11">
         <f>Hoja2!E4</f>
-        <v>1115.19</v>
+        <v>1500</v>
       </c>
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
     </row>
     <row r="4" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C4" s="2" t="s">
-        <v>13</v>
+        <v>35</v>
       </c>
       <c r="D4" s="11">
         <f>Hoja2!E6</f>
-        <v>67.33</v>
+        <v>75</v>
       </c>
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
     </row>
     <row r="5" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C5" s="2" t="s">
-        <v>14</v>
+        <v>38</v>
       </c>
       <c r="D5" s="11">
         <f>Hoja2!E7</f>
-        <v>26.04</v>
+        <v>48</v>
       </c>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
     </row>
     <row r="6" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C6" s="2"/>
+      <c r="C6" s="2" t="s">
+        <v>39</v>
+      </c>
       <c r="D6" s="11">
         <f>Hoja2!E8</f>
-        <v>0</v>
+        <v>145</v>
       </c>
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
@@ -630,7 +641,7 @@
       </c>
       <c r="D7" s="11">
         <f>Hoja2!E9</f>
-        <v>0</v>
+        <v>67.5</v>
       </c>
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
@@ -648,8 +659,8 @@
         <v>10</v>
       </c>
       <c r="D9" s="11">
-        <f>D3/6</f>
-        <v>185.86500000000001</v>
+        <f>(D3+D4)/6</f>
+        <v>262.5</v>
       </c>
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
@@ -678,8 +689,8 @@
         <v>6</v>
       </c>
       <c r="D13" s="11">
-        <f>D3+D4+D5+D9+(IF(D10&gt;(26.67*2),D10-(26.67*2),0))</f>
-        <v>1394.425</v>
+        <f>D3+D4+D5+D6+D9+(IF(D10&gt;(26.67*2),D10-(26.67*2),0))</f>
+        <v>2030.5</v>
       </c>
       <c r="E13" s="3"/>
       <c r="F13" s="3"/>
@@ -690,7 +701,7 @@
       </c>
       <c r="D14" s="11">
         <f>D13+D7+D8</f>
-        <v>1394.425</v>
+        <v>2098</v>
       </c>
       <c r="E14" s="3"/>
       <c r="F14" s="3"/>
@@ -701,7 +712,7 @@
       </c>
       <c r="D15" s="11">
         <f>D7</f>
-        <v>0</v>
+        <v>67.5</v>
       </c>
       <c r="E15" s="1"/>
       <c r="F15" s="1"/>
@@ -728,8 +739,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5EA8BEC2-E289-4038-A182-9F995A73E1A4}">
   <dimension ref="C3:E32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+    <sheetView tabSelected="1" topLeftCell="B5" workbookViewId="0">
+      <selection activeCell="I29" sqref="I29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -751,7 +762,7 @@
       </c>
       <c r="D4" s="6"/>
       <c r="E4" s="10">
-        <v>1115.19</v>
+        <v>1500</v>
       </c>
     </row>
     <row r="5" spans="3:5" x14ac:dyDescent="0.3">
@@ -763,38 +774,43 @@
     </row>
     <row r="6" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C6" t="s">
-        <v>13</v>
+        <v>35</v>
       </c>
       <c r="D6" s="6"/>
       <c r="E6" s="10">
-        <v>67.33</v>
+        <v>75</v>
       </c>
     </row>
     <row r="7" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C7" t="s">
-        <v>14</v>
+        <v>36</v>
       </c>
       <c r="D7" s="6"/>
       <c r="E7" s="10">
-        <v>26.04</v>
+        <v>48</v>
       </c>
     </row>
     <row r="8" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C8" t="s">
+        <v>37</v>
+      </c>
       <c r="D8" s="6"/>
-      <c r="E8" s="10"/>
+      <c r="E8" s="10">
+        <v>145</v>
+      </c>
     </row>
     <row r="9" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C9" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D9" s="6"/>
       <c r="E9" s="10">
-        <v>0</v>
+        <v>67.5</v>
       </c>
     </row>
     <row r="10" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C10" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D10" s="6"/>
       <c r="E10" s="10">
@@ -803,16 +819,17 @@
     </row>
     <row r="11" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C11" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D11" s="6"/>
       <c r="E11" s="10">
-        <v>0</v>
+        <f>(E4+E6)/6</f>
+        <v>262.5</v>
       </c>
     </row>
     <row r="12" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C12" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D12" s="6"/>
       <c r="E12" s="10">
@@ -821,14 +838,14 @@
     </row>
     <row r="13" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C13" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D13" s="6"/>
       <c r="E13" s="4"/>
     </row>
     <row r="14" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C14" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D14" s="6"/>
       <c r="E14" s="10">
@@ -837,7 +854,7 @@
     </row>
     <row r="15" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C15" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D15" s="6"/>
       <c r="E15" s="10">
@@ -846,7 +863,7 @@
     </row>
     <row r="16" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C16" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D16" s="6"/>
       <c r="E16" s="10">
@@ -855,7 +872,7 @@
     </row>
     <row r="17" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C17" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D17" s="6"/>
       <c r="E17" s="10">
@@ -864,12 +881,12 @@
     </row>
     <row r="18" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C18" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D18" s="6"/>
       <c r="E18" s="10">
         <f>SUM(E4:E17)</f>
-        <v>1208.56</v>
+        <v>2098</v>
       </c>
     </row>
     <row r="19" spans="3:5" x14ac:dyDescent="0.3">
@@ -879,86 +896,86 @@
     </row>
     <row r="20" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C20" s="5" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D20" s="8" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="E20" s="6"/>
     </row>
     <row r="21" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C21" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D21" s="9">
         <v>4.7E-2</v>
       </c>
       <c r="E21" s="10">
         <f>Hoja1!D13*D21</f>
-        <v>65.537975000000003</v>
+        <v>95.433499999999995</v>
       </c>
     </row>
     <row r="22" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C22" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D22" s="9">
         <v>1.55E-2</v>
       </c>
       <c r="E22" s="10">
         <f>Hoja1!D14*D22</f>
-        <v>21.613587499999998</v>
+        <v>32.518999999999998</v>
       </c>
     </row>
     <row r="23" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C23" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D23" s="9">
         <v>1E-3</v>
       </c>
       <c r="E23" s="10">
         <f>Hoja1!D14*D23</f>
-        <v>1.394425</v>
+        <v>2.0979999999999999</v>
       </c>
     </row>
     <row r="24" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C24" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D24" s="9">
         <v>4.7E-2</v>
       </c>
       <c r="E24" s="10">
         <f>Hoja1!D15*D24</f>
-        <v>0</v>
+        <v>3.1724999999999999</v>
       </c>
     </row>
     <row r="25" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C25" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D25" s="6"/>
       <c r="E25" s="10">
         <f>SUM(E21:E24)</f>
-        <v>88.545987499999995</v>
+        <v>133.22300000000001</v>
       </c>
     </row>
     <row r="26" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C26" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D26" s="9">
-        <v>0.02</v>
+        <v>0.1</v>
       </c>
       <c r="E26" s="10">
         <f>SUM(E4:E12)*D26</f>
-        <v>24.171199999999999</v>
+        <v>209.8</v>
       </c>
     </row>
     <row r="27" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C27" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D27" s="6"/>
       <c r="E27" s="10">
@@ -967,7 +984,7 @@
     </row>
     <row r="28" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C28" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D28" s="6"/>
       <c r="E28" s="10">
@@ -976,7 +993,7 @@
     </row>
     <row r="29" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C29" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D29" s="6"/>
       <c r="E29" s="10">
@@ -985,12 +1002,12 @@
     </row>
     <row r="30" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C30" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D30" s="6"/>
       <c r="E30" s="10">
         <f>SUM(E25:E29)</f>
-        <v>112.71718749999999</v>
+        <v>343.02300000000002</v>
       </c>
     </row>
     <row r="31" spans="3:5" x14ac:dyDescent="0.3">
@@ -1000,16 +1017,16 @@
     </row>
     <row r="32" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C32" s="2" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D32" s="6"/>
       <c r="E32" s="10">
         <f>E18-E30</f>
-        <v>1095.8428125</v>
+        <v>1754.9769999999999</v>
       </c>
     </row>
   </sheetData>
-  <sheetProtection sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
+  <sheetProtection selectLockedCells="1"/>
   <dataValidations count="2">
     <dataValidation type="textLength" errorStyle="information" operator="lessThan" allowBlank="1" showInputMessage="1" sqref="E5 E13" xr:uid="{DFAA6B4A-027D-479E-99F3-8C3016310E54}">
       <formula1>99999</formula1>

</xml_diff>